<commit_message>
removed launch hotkey + modified data
</commit_message>
<xml_diff>
--- a/data3.xlsx
+++ b/data3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leocr\Desktop\bot-autohotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70BA45A-D020-4A75-A5F3-01CD0B82D65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC569742-8488-4D2E-9127-2ECB4865A577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="60" windowWidth="23280" windowHeight="12900" xr2:uid="{B887B182-F6ED-4213-9DB9-E78F9A5CD812}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B887B182-F6ED-4213-9DB9-E78F9A5CD812}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>Profitez de l’expertise d'Équipes de Déménagement</t>
   </si>
   <si>
-    <t>Nous mobilisons une équipe de Déménageurs Qualifiés</t>
-  </si>
-  <si>
     <t>En toute sécurité, on vous Déménage</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
 ⚠️Le prix est suivant la formule et la distance  ⚠️
 ⚠️ Le prix est suivant la formule et la distance  ⚠️
 ⚠️ Le prix est suivant la formule et la distance  ⚠️</t>
+  </si>
+  <si>
+    <t>leboncoin.fr/deposer-une-annonce</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -763,10 +763,10 @@
     </row>
     <row r="6" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="7" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -797,10 +797,10 @@
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -814,10 +814,10 @@
     </row>
     <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -831,10 +831,10 @@
     </row>
     <row r="10" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -851,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>

</xml_diff>